<commit_message>
Avanço do codigo de preparação e testes
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Resultado consulta.xlsx
+++ b/Correcao EPROC/Resultado consulta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,17 +503,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5009993-03.2012.8.21.0001</t>
+          <t>5009222-59.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0390818-43.2012.8.21.0001</t>
+          <t>0324997-29.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CIV.33244.01</t>
+          <t>CIV.27790.01</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -528,17 +528,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5009871-87.2012.8.21.0001</t>
+          <t>5011355-74.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0350094-94.2012.8.21.0001</t>
+          <t>0301050-43.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CIV.33239.01</t>
+          <t>CIV.32060.01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -553,17 +553,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5017259-75.2011.8.21.0001</t>
+          <t>5164293-68.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0418962-61.2011.8.21.0001</t>
+          <t>5052584-96.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CIV.29138.01</t>
+          <t>CIV.36785.01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -578,17 +578,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5029266-60.2015.8.21.0001</t>
+          <t>5034678-11.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0229724-81.2015.8.21.0001</t>
+          <t>0366891-82.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CIV.18373.01</t>
+          <t>CIV.43532.01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -603,17 +603,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5033756-96.2013.8.21.0001</t>
+          <t>5005050-83.2017.8.21.0027</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0051408-17.2013.8.21.0001</t>
+          <t>9006750-26.2017.8.21.0027</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CIV.18528.01</t>
+          <t>CIV.36338.01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -628,17 +628,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5033756-96.2013.8.21.0001</t>
+          <t>5005051-68.2017.8.21.0027</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0051408-17.2013.8.21.0001</t>
+          <t>9006808-29.2017.8.21.0027</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CIV.18528.01</t>
+          <t>CIV.36301.01</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -653,17 +653,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5164293-68.2022.8.21.0001</t>
+          <t>5005049-98.2017.8.21.0027</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5052584-96.2020.8.21.0001</t>
+          <t>9007658-83.2017.8.21.0027</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CIV.36785.01</t>
+          <t>CIV.36285.01</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -678,17 +678,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5011774-94.2011.8.21.0001</t>
+          <t>5005048-16.2017.8.21.0027</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0305839-85.2011.8.21.0001</t>
+          <t>9007049-03.2017.8.21.0027</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CIV.30164.01</t>
+          <t>CIV.36330.01</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -703,17 +703,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5018623-68.2020.8.21.0033</t>
+          <t>5040819-16.2021.8.21.0027</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0005691-67.2021.8.21.9000</t>
+          <t>9002011-68.2021.8.21.0027</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CIV.17056.02</t>
+          <t>CIV.43956.01</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -728,17 +728,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5005050-83.2017.8.21.0027</t>
+          <t>5034672-67.2012.8.21.0001</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9006750-26.2017.8.21.0027</t>
+          <t>0329535-19.2012.8.21.0001</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CIV.36338.01</t>
+          <t>CIV.30902.01</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -753,17 +753,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5005051-68.2017.8.21.0027</t>
+          <t>5021122-68.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>9006808-29.2017.8.21.0027</t>
+          <t>0366965-68.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CIV.36301.01</t>
+          <t>CIV.12636.01</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -778,17 +778,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5005049-98.2017.8.21.0027</t>
+          <t>5021122-68.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>9007658-83.2017.8.21.0027</t>
+          <t>0366965-68.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CIV.36285.01</t>
+          <t>CIV.12636.01</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -803,17 +803,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5005048-16.2017.8.21.0027</t>
+          <t>5100739-96.2021.8.21.0001</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>9007049-03.2017.8.21.0027</t>
+          <t>5020041-40.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CIV.36330.01</t>
+          <t>CIV.35465.01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -828,17 +828,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5040819-16.2021.8.21.0027</t>
+          <t>5021493-03.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>9002011-68.2021.8.21.0027</t>
+          <t>0330513-30.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CIV.43956.01</t>
+          <t>CIV.13775.01</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -853,17 +853,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5034672-67.2012.8.21.0001</t>
+          <t>5001340-37.2018.8.21.0054</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0329535-19.2012.8.21.0001</t>
+          <t>0010601-11.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CIV.30902.01</t>
+          <t>CIV.34884.02</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -878,17 +878,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5021122-68.2013.8.21.0001</t>
+          <t>5015486-29.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0366965-68.2013.8.21.0001</t>
+          <t>0476301-12.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CIV.12636.01</t>
+          <t>CIV.03796.01</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -903,17 +903,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5021122-68.2013.8.21.0001</t>
+          <t>5015486-29.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0366965-68.2013.8.21.0001</t>
+          <t>0476301-12.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>CIV.12636.01</t>
+          <t>CIV.03796.01</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -928,20 +928,995 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5100739-96.2021.8.21.0001</t>
+          <t>5039762-80.2017.8.21.0001</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5020041-40.2020.8.21.0001</t>
+          <t>0140217-41.2017.8.21.0001</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CIV.35465.01</t>
+          <t>CIV.37500.01</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>5123070-43.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0156245-16.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>CIV.37821.01</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5039761-95.2017.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0208080-14.2017.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>CIV.00585.01</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5111935-34.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>9026683-92.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>CIV.12633.01</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>5111861-77.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>9026274-19.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>CIV.00342.01</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5111845-26.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>9024067-47.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>CIV.34718.01</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5111932-79.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>9026423-15.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CIV.00343.01</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5111929-27.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>9024645-10.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>CIV.01839.01</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5111816-73.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>9029042-15.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>CIV.16470.01</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5111835-79.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>9023325-22.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>CIV.33830.01</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>5111822-80.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>9030447-86.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>CIV.16515.01</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>5111790-75.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>9025668-88.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>CIV.34610.01</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>5111810-66.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>9022457-44.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>CIV.03811.01</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>5111830-57.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>9061633-30.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>CIV.07454.01</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>5111831-42.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>9029579-11.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CIV.35367.01</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>5111815-88.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>9029039-60.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>CIV.39670.01</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>5111787-23.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>9025911-32.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>CIV.39600.01</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>5111799-37.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>9025028-85.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>CIV.15912.01</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>5111813-21.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>9029035-23.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>CIV.16479.01</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>5111825-35.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>9026575-63.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>CIV.39624.01</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>5111759-55.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>9060965-59.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>CIV.07301.01</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>5111741-34.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>9025693-04.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>CIV.03810.01</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>5111776-91.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>9023851-86.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>CIV.33796.01</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>5111778-61.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>9061623-83.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>CIV.07449.01</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>5111744-86.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>9025890-56.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>CIV.34364.01</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>5111785-53.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>9025909-62.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>CIV.34524.01</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>5111737-94.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>9025685-27.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>CIV.34600.01</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>5111770-84.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>9055671-26.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>CIV.04346.01</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>5111779-46.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>9059856-10.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>CIV.06530.01</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>5111736-12.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>9023259-42.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>CIV.07304.01</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>5111739-64.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>9025691-34.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>CIV.15914.01</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>5111745-71.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>9025891-41.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>CIV.39592.01</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>5111764-77.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>9061411-62.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>CIV.07283.01</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>5111728-35.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>9025865-43.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>CIV.12624.01</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>5111691-08.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>9022700-85.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>CIV.15836.01</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>5111708-44.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>9019634-97.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>CIV.15806.01</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>5111695-45.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>9021607-87.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>CIV.15778.01</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>5111699-82.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>9060613-04.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>CIV.06950.01</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>5111706-74.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>9023030-82.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>CIV.39564.01</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>originario_principal</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>5111705-89.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>9023029-97.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>CIV.15771.01</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>originario_principal</t>
         </is>

</xml_diff>

<commit_message>
Correção da preparação de dados
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Resultado consulta.xlsx
+++ b/Correcao EPROC/Resultado consulta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,17 +453,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5216394-82.2022.8.21.0001</t>
+          <t>5157435-21.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5047561-72.2020.8.21.0001</t>
+          <t>5032648-85.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CIV.36761.01</t>
+          <t>CIV.36083.01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -478,17 +478,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5164586-38.2022.8.21.0001</t>
+          <t>5006597-19.2022.8.21.0049</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5006043-05.2020.8.21.0001</t>
+          <t>5002821-79.2020.8.21.0049</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CIV.35117.01</t>
+          <t>CIV.36217.01</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -503,17 +503,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5009222-59.2011.8.21.0001</t>
+          <t>5167764-92.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0324997-29.2011.8.21.0001</t>
+          <t>5029537-93.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CIV.27790.01</t>
+          <t>CIV.35613.01</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -528,17 +528,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5011355-74.2011.8.21.0001</t>
+          <t>5172099-57.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0301050-43.2011.8.21.0001</t>
+          <t>5032767-46.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CIV.32060.01</t>
+          <t>CIV.36084.01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -553,17 +553,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5164293-68.2022.8.21.0001</t>
+          <t>5030909-28.2022.8.21.0027</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5052584-96.2020.8.21.0001</t>
+          <t>5004621-14.2020.8.21.0027</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CIV.36785.01</t>
+          <t>CIV.35884.01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -578,17 +578,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5034678-11.2011.8.21.0001</t>
+          <t>5006597-19.2022.8.21.0049</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0366891-82.2011.8.21.0001</t>
+          <t>5002821-79.2020.8.21.0049</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CIV.43532.01</t>
+          <t>CIV.36217.01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -603,17 +603,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5005050-83.2017.8.21.0027</t>
+          <t>5033570-92.2022.8.21.0022</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9006750-26.2017.8.21.0027</t>
+          <t>5008789-45.2018.8.21.0022</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CIV.36338.01</t>
+          <t>CIV.03068.03</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -628,17 +628,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5005051-68.2017.8.21.0027</t>
+          <t>5033570-92.2022.8.21.0022</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9006808-29.2017.8.21.0027</t>
+          <t>5008789-45.2018.8.21.0022</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CIV.36301.01</t>
+          <t>CIV.03068.03</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -653,17 +653,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5005049-98.2017.8.21.0027</t>
+          <t>5001180-41.2018.8.21.0012</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>9007658-83.2017.8.21.0027</t>
+          <t>0013778-46.2020.8.21.9000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CIV.36285.01</t>
+          <t>CIV.34844.02</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -678,17 +678,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5005048-16.2017.8.21.0027</t>
+          <t>5016732-06.2023.8.21.0001</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9007049-03.2017.8.21.0027</t>
+          <t>0022795-65.2005.8.21.0001</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CIV.36330.01</t>
+          <t>CIV.32871.01</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -703,17 +703,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5040819-16.2021.8.21.0027</t>
+          <t>5016732-06.2023.8.21.0001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9002011-68.2021.8.21.0027</t>
+          <t>0022795-65.2005.8.21.0001</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CIV.43956.01</t>
+          <t>CIV.32871.01</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -728,17 +728,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5034672-67.2012.8.21.0001</t>
+          <t>5002010-65.2020.8.21.0067</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0329535-19.2012.8.21.0001</t>
+          <t>9000544-65.2020.8.21.0067</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CIV.30902.01</t>
+          <t>CIV.36915.01</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -753,17 +753,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5021122-68.2013.8.21.0001</t>
+          <t>5000993-62.2018.8.21.0067</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0366965-68.2013.8.21.0001</t>
+          <t>9000840-58.2018.8.21.0067</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CIV.12636.01</t>
+          <t>CIV.35834.01</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -778,17 +778,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5021122-68.2013.8.21.0001</t>
+          <t>5033890-89.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0366965-68.2013.8.21.0001</t>
+          <t>0380267-33.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CIV.12636.01</t>
+          <t>CIV.19910.01</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -803,17 +803,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5100739-96.2021.8.21.0001</t>
+          <t>5033712-43.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5020041-40.2020.8.21.0001</t>
+          <t>0314096-94.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CIV.35465.01</t>
+          <t>CIV.19755.01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -828,17 +828,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5021493-03.2011.8.21.0001</t>
+          <t>5010009-54.2012.8.21.0001</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0330513-30.2011.8.21.0001</t>
+          <t>0266239-23.2012.8.21.0001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CIV.13775.01</t>
+          <t>CIV.30752.01</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -853,17 +853,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5001340-37.2018.8.21.0054</t>
+          <t>5033709-88.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0010601-11.2019.8.21.9000</t>
+          <t>0361665-91.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CIV.34884.02</t>
+          <t>CIV.20812.01</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -878,17 +878,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5015486-29.2010.8.21.0001</t>
+          <t>5027774-33.2015.8.21.0001</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0476301-12.2010.8.21.0001</t>
+          <t>0098129-56.2015.8.21.0001</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CIV.03796.01</t>
+          <t>CIV.19753.01</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -903,17 +903,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5015486-29.2010.8.21.0001</t>
+          <t>5033650-03.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0476301-12.2010.8.21.0001</t>
+          <t>0352497-65.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>CIV.03796.01</t>
+          <t>CIV.20814.01</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -928,17 +928,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5039762-80.2017.8.21.0001</t>
+          <t>5012011-26.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0140217-41.2017.8.21.0001</t>
+          <t>0192467-56.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CIV.37500.01</t>
+          <t>CIV.18708.01</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -953,17 +953,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5123070-43.2019.8.21.0001</t>
+          <t>5012011-26.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0156245-16.2019.8.21.0001</t>
+          <t>0192467-56.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>CIV.37821.01</t>
+          <t>CIV.18708.01</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -978,17 +978,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5039761-95.2017.8.21.0001</t>
+          <t>5001222-27.2018.8.21.0130</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0208080-14.2017.8.21.0001</t>
+          <t>0064994-80.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>CIV.00585.01</t>
+          <t>CIV.02989.02</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1003,17 +1003,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5111935-34.2019.8.21.0001</t>
+          <t>5001222-27.2018.8.21.0130</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>9026683-92.2019.8.21.0001</t>
+          <t>0064994-80.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CIV.12633.01</t>
+          <t>CIV.02989.02</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1028,17 +1028,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5111861-77.2019.8.21.0001</t>
+          <t>5162162-23.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>9026274-19.2019.8.21.0001</t>
+          <t>5013305-06.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CIV.00342.01</t>
+          <t>CIV.35301.01</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1053,17 +1053,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5111845-26.2019.8.21.0001</t>
+          <t>5033540-72.2012.8.21.0001</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>9024067-47.2019.8.21.0001</t>
+          <t>0245475-16.2012.8.21.0001</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CIV.34718.01</t>
+          <t>CIV.19909.01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1078,17 +1078,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5111932-79.2019.8.21.0001</t>
+          <t>5028177-02.2015.8.21.0001</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>9026423-15.2019.8.21.0001</t>
+          <t>0104387-82.2015.8.21.0001</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>CIV.00343.01</t>
+          <t>CIV.11768.01</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1103,17 +1103,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5111929-27.2019.8.21.0001</t>
+          <t>5011672-14.2007.8.21.0001</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>9024645-10.2019.8.21.0001</t>
+          <t>0813081-77.2007.8.21.0001</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>CIV.01839.01</t>
+          <t>CIV.01858.01</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1128,17 +1128,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5111816-73.2019.8.21.0001</t>
+          <t>5015372-90.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>9029042-15.2019.8.21.0001</t>
+          <t>3015561-05.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>CIV.16470.01</t>
+          <t>CIV.08551.01</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1153,17 +1153,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5111835-79.2019.8.21.0001</t>
+          <t>5033872-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>9023325-22.2019.8.21.0001</t>
+          <t>0051176-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>CIV.33830.01</t>
+          <t>CIV.09344.01</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1178,17 +1178,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5111822-80.2019.8.21.0001</t>
+          <t>5033872-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>9030447-86.2019.8.21.0001</t>
+          <t>0051176-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>CIV.16515.01</t>
+          <t>CIV.09344.01</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1203,17 +1203,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5111790-75.2019.8.21.0001</t>
+          <t>5033872-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>9025668-88.2019.8.21.0001</t>
+          <t>0051176-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>CIV.34610.01</t>
+          <t>CIV.09344.01</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1228,17 +1228,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5111810-66.2019.8.21.0001</t>
+          <t>5033872-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>9022457-44.2019.8.21.0001</t>
+          <t>0051176-05.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CIV.03811.01</t>
+          <t>CIV.09344.01</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1253,17 +1253,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5111830-57.2019.8.21.0001</t>
+          <t>5015383-22.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>9061633-30.2019.8.21.0001</t>
+          <t>2549411-10.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>CIV.07454.01</t>
+          <t>CIV.18592.01</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1278,17 +1278,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5111831-42.2019.8.21.0001</t>
+          <t>5015383-22.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>9029579-11.2019.8.21.0001</t>
+          <t>2549411-10.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>CIV.35367.01</t>
+          <t>CIV.18592.01</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1303,620 +1303,20 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5111815-88.2019.8.21.0001</t>
+          <t>5001283-19.2018.8.21.0054</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>9029039-60.2019.8.21.0001</t>
+          <t>0035364-76.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>CIV.39670.01</t>
+          <t>CIV.06068.02</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>5111787-23.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>9025911-32.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>CIV.39600.01</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>5111799-37.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>9025028-85.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>CIV.15912.01</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>5111813-21.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>9029035-23.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>CIV.16479.01</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>5111825-35.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>9026575-63.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>CIV.39624.01</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>5111759-55.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>9060965-59.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>CIV.07301.01</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>5111741-34.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>9025693-04.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>CIV.03810.01</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>5111776-91.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>9023851-86.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>CIV.33796.01</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>5111778-61.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>9061623-83.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>CIV.07449.01</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>5111744-86.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>9025890-56.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>CIV.34364.01</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>5111785-53.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>9025909-62.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>CIV.34524.01</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>5111737-94.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>9025685-27.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>CIV.34600.01</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>5111770-84.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>9055671-26.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>CIV.04346.01</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>5111779-46.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>9059856-10.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>CIV.06530.01</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>5111736-12.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>9023259-42.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>CIV.07304.01</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>5111739-64.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>9025691-34.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>CIV.15914.01</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>5111745-71.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>9025891-41.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>CIV.39592.01</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>5111764-77.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>9061411-62.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>CIV.07283.01</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>5111728-35.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>9025865-43.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>CIV.12624.01</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>5111691-08.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>9022700-85.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>CIV.15836.01</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>5111708-44.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>9019634-97.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>CIV.15806.01</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>5111695-45.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>9021607-87.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>CIV.15778.01</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>5111699-82.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>9060613-04.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>CIV.06950.01</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>5111706-74.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>9023030-82.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>CIV.39564.01</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>originario_principal</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>5111705-89.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>9023029-97.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>CIV.15771.01</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
         <is>
           <t>originario_principal</t>
         </is>

</xml_diff>